<commit_message>
Update Documentation and Commit Current Changes
</commit_message>
<xml_diff>
--- a/Documentation/BioRubeBot_ProductBackLog_Su16.xlsx
+++ b/Documentation/BioRubeBot_ProductBackLog_Su16.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="38">
   <si>
     <t>Task Name</t>
   </si>
@@ -126,6 +121,18 @@
   </si>
   <si>
     <t>Add tutorial that shows how to play the game, make moves in the game, change background color, etc.</t>
+  </si>
+  <si>
+    <t>Sprint 3</t>
+  </si>
+  <si>
+    <t>Add menu with game pieces (Free Play Level)</t>
+  </si>
+  <si>
+    <t>Add functionality with game pieces on the cell  (Free Play Level)</t>
+  </si>
+  <si>
+    <t>Allow game pieces to interact when the play button is clicked  (Free Play Level)</t>
   </si>
 </sst>
 </file>
@@ -458,7 +465,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -466,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,7 +554,7 @@
         <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -602,7 +609,7 @@
         <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -619,7 +626,7 @@
         <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -630,7 +637,7 @@
         <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -641,7 +648,7 @@
         <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -652,7 +659,7 @@
         <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -663,7 +670,7 @@
         <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -674,7 +681,7 @@
         <v>32</v>
       </c>
       <c r="C19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -685,11 +692,56 @@
         <v>33</v>
       </c>
       <c r="C20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="7"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="7"/>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>